<commit_message>
updated Belgium and Fig 4
</commit_message>
<xml_diff>
--- a/data/dris/raw/efsa/EFSA_2018_upper_limits.xlsx
+++ b/data/dris/raw/efsa/EFSA_2018_upper_limits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/nutrition/subnational_nutrient_distributions/data/dris/raw/efsa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394F7A08-81C3-3040-A979-F236A43AA554}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4579F11B-33D4-1345-BD76-4863BE38E8F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1470,7 +1470,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>